<commit_message>
add weight memory calculate
</commit_message>
<xml_diff>
--- a/metrics/qwen3-32B_prefill.xlsx
+++ b/metrics/qwen3-32B_prefill.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,7 @@
     <col width="12" customWidth="1" min="14" max="14"/>
     <col width="12" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -573,6 +574,11 @@
           <t>占比(%)</t>
         </is>
       </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>权重/单卡alllayers</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -633,6 +639,9 @@
       <c r="P4" s="6" t="n">
         <v>6.84</v>
       </c>
+      <c r="Q4" s="4" t="n">
+        <v>838860800</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -693,6 +702,9 @@
       <c r="P5" s="6" t="n">
         <v>5.47</v>
       </c>
+      <c r="Q5" s="4" t="n">
+        <v>671088640</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -753,6 +765,9 @@
       <c r="P6" s="6" t="n">
         <v>34.21</v>
       </c>
+      <c r="Q6" s="4" t="n">
+        <v>4194304000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -813,6 +828,9 @@
       <c r="P7" s="6" t="n">
         <v>17.11</v>
       </c>
+      <c r="Q7" s="4" t="n">
+        <v>2097152000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -873,6 +891,9 @@
       <c r="P8" s="6" t="n">
         <v>4.38</v>
       </c>
+      <c r="Q8" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -933,6 +954,9 @@
       <c r="P9" s="6" t="n">
         <v>0.55</v>
       </c>
+      <c r="Q9" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -993,6 +1017,9 @@
       <c r="P10" s="6" t="n">
         <v>15.72</v>
       </c>
+      <c r="Q10" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -1053,6 +1080,9 @@
       <c r="P11" s="6" t="n">
         <v>15.72</v>
       </c>
+      <c r="Q11" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="inlineStr">
@@ -1126,9 +1156,19 @@
         <v>19990.959</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>权重显存/单卡(GB)</t>
+        </is>
+      </c>
+      <c r="B25" s="8" t="n">
+        <v>7.266</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>